<commit_message>
Button to submit added, efficiency of captcha increased
</commit_message>
<xml_diff>
--- a/result/student_marks.xlsx
+++ b/result/student_marks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:J1"/>
+  <dimension ref="A1:AL4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,47 +436,595 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>USN</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Internals</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Externals</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Internals.1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Externals.1</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Total.1</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks.1</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Internals.2</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Externals.2</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Total.2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks.2</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Internals.3</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Externals.3</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Total.3</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks.3</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Internals.4</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Externals.4</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Total.4</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks.4</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Internals.5</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Externals.5</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Total.5</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks.5</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Internals.6</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Externals.6</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Total.6</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks.6</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Internals.7</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Externals.7</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Total.7</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks.7</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Internals.8</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Externals.8</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Total.8</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Remarks.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>1AM18CS002</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>52.1</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>P.1</t>
+      <c r="C2" t="n">
+        <v>22</v>
+      </c>
+      <c r="D2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E2" t="n">
+        <v>52</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>24</v>
+      </c>
+      <c r="H2" t="n">
+        <v>28</v>
+      </c>
+      <c r="I2" t="n">
+        <v>52</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>27</v>
+      </c>
+      <c r="L2" t="n">
+        <v>9</v>
+      </c>
+      <c r="M2" t="n">
+        <v>36</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>34</v>
+      </c>
+      <c r="P2" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>49</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="S2" t="n">
+        <v>24</v>
+      </c>
+      <c r="T2" t="n">
+        <v>13</v>
+      </c>
+      <c r="U2" t="n">
+        <v>37</v>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="W2" t="n">
+        <v>37</v>
+      </c>
+      <c r="X2" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>58</v>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AA2" t="n">
+        <v>35</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>62</v>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AE2" t="n">
+        <v>35</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>39</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>74</v>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AI2" t="n">
+        <v>37</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>24</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>61</v>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1AM18CS006</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>25</v>
+      </c>
+      <c r="D3" t="n">
+        <v>37</v>
+      </c>
+      <c r="E3" t="n">
+        <v>62</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>18</v>
+      </c>
+      <c r="H3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I3" t="n">
+        <v>41</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>23</v>
+      </c>
+      <c r="L3" t="n">
+        <v>21</v>
+      </c>
+      <c r="M3" t="n">
+        <v>44</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>29</v>
+      </c>
+      <c r="P3" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>41</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>16</v>
+      </c>
+      <c r="T3" t="n">
+        <v>21</v>
+      </c>
+      <c r="U3" t="n">
+        <v>37</v>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="W3" t="n">
+        <v>20</v>
+      </c>
+      <c r="X3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>41</v>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AA3" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>59</v>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AE3" t="n">
+        <v>40</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>39</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>79</v>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AI3" t="n">
+        <v>37</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>58</v>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1AM18CS099</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>19</v>
+      </c>
+      <c r="D4" t="n">
+        <v>25</v>
+      </c>
+      <c r="E4" t="n">
+        <v>44</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>22</v>
+      </c>
+      <c r="H4" t="n">
+        <v>16</v>
+      </c>
+      <c r="I4" t="n">
+        <v>38</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>22</v>
+      </c>
+      <c r="L4" t="n">
+        <v>21</v>
+      </c>
+      <c r="M4" t="n">
+        <v>43</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>29</v>
+      </c>
+      <c r="P4" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>37</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>20</v>
+      </c>
+      <c r="T4" t="n">
+        <v>21</v>
+      </c>
+      <c r="U4" t="n">
+        <v>41</v>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="W4" t="n">
+        <v>19</v>
+      </c>
+      <c r="X4" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="AA4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>59</v>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AE4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>45</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>75</v>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AI4" t="n">
+        <v>37</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>67</v>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>P</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
flask integration with frontend
</commit_message>
<xml_diff>
--- a/result/student_marks.xlsx
+++ b/result/student_marks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL4"/>
+  <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1028,6 +1028,278 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1AM18CS010</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>26</v>
+      </c>
+      <c r="D5" t="n">
+        <v>29</v>
+      </c>
+      <c r="E5" t="n">
+        <v>55</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>28</v>
+      </c>
+      <c r="H5" t="n">
+        <v>21</v>
+      </c>
+      <c r="I5" t="n">
+        <v>49</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>23</v>
+      </c>
+      <c r="L5" t="n">
+        <v>35</v>
+      </c>
+      <c r="M5" t="n">
+        <v>58</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>34</v>
+      </c>
+      <c r="P5" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>49</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>33</v>
+      </c>
+      <c r="T5" t="n">
+        <v>18</v>
+      </c>
+      <c r="U5" t="n">
+        <v>51</v>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="W5" t="n">
+        <v>21</v>
+      </c>
+      <c r="X5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>54</v>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AA5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>66</v>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AE5" t="n">
+        <v>25</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>41</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>66</v>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AI5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>29</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>66</v>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1AM18CS028</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>20</v>
+      </c>
+      <c r="D6" t="n">
+        <v>21</v>
+      </c>
+      <c r="E6" t="n">
+        <v>41</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>21</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>21</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>22</v>
+      </c>
+      <c r="L6" t="n">
+        <v>8</v>
+      </c>
+      <c r="M6" t="n">
+        <v>30</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>18</v>
+      </c>
+      <c r="P6" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>33</v>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>19</v>
+      </c>
+      <c r="T6" t="n">
+        <v>9</v>
+      </c>
+      <c r="U6" t="n">
+        <v>28</v>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="W6" t="n">
+        <v>17</v>
+      </c>
+      <c r="X6" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>26</v>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="AA6" t="n">
+        <v>33</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>60</v>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AE6" t="n">
+        <v>25</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>38</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>63</v>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="AI6" t="n">
+        <v>37</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>63</v>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upload, run adn download results integrated with backend
</commit_message>
<xml_diff>
--- a/result/student_marks.xlsx
+++ b/result/student_marks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL6"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -756,550 +756,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1AM18CS006</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>25</v>
-      </c>
-      <c r="D3" t="n">
-        <v>37</v>
-      </c>
-      <c r="E3" t="n">
-        <v>62</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>18</v>
-      </c>
-      <c r="H3" t="n">
-        <v>23</v>
-      </c>
-      <c r="I3" t="n">
-        <v>41</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>23</v>
-      </c>
-      <c r="L3" t="n">
-        <v>21</v>
-      </c>
-      <c r="M3" t="n">
-        <v>44</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="O3" t="n">
-        <v>29</v>
-      </c>
-      <c r="P3" t="n">
-        <v>12</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>41</v>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="S3" t="n">
-        <v>16</v>
-      </c>
-      <c r="T3" t="n">
-        <v>21</v>
-      </c>
-      <c r="U3" t="n">
-        <v>37</v>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="W3" t="n">
-        <v>20</v>
-      </c>
-      <c r="X3" t="n">
-        <v>21</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>41</v>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="AA3" t="n">
-        <v>32</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>27</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>59</v>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="AE3" t="n">
-        <v>40</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>39</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>79</v>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="AI3" t="n">
-        <v>37</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>21</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>58</v>
-      </c>
-      <c r="AL3" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1AM18CS099</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>19</v>
-      </c>
-      <c r="D4" t="n">
-        <v>25</v>
-      </c>
-      <c r="E4" t="n">
-        <v>44</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>22</v>
-      </c>
-      <c r="H4" t="n">
-        <v>16</v>
-      </c>
-      <c r="I4" t="n">
-        <v>38</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>22</v>
-      </c>
-      <c r="L4" t="n">
-        <v>21</v>
-      </c>
-      <c r="M4" t="n">
-        <v>43</v>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="O4" t="n">
-        <v>29</v>
-      </c>
-      <c r="P4" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>37</v>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
-        <v>20</v>
-      </c>
-      <c r="T4" t="n">
-        <v>21</v>
-      </c>
-      <c r="U4" t="n">
-        <v>41</v>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="W4" t="n">
-        <v>19</v>
-      </c>
-      <c r="X4" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>33</v>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="AA4" t="n">
-        <v>32</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>27</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>59</v>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="AE4" t="n">
-        <v>30</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>45</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>75</v>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="AI4" t="n">
-        <v>37</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>30</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>67</v>
-      </c>
-      <c r="AL4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1AM18CS010</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>26</v>
-      </c>
-      <c r="D5" t="n">
-        <v>29</v>
-      </c>
-      <c r="E5" t="n">
-        <v>55</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>28</v>
-      </c>
-      <c r="H5" t="n">
-        <v>21</v>
-      </c>
-      <c r="I5" t="n">
-        <v>49</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>23</v>
-      </c>
-      <c r="L5" t="n">
-        <v>35</v>
-      </c>
-      <c r="M5" t="n">
-        <v>58</v>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="O5" t="n">
-        <v>34</v>
-      </c>
-      <c r="P5" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>49</v>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="S5" t="n">
-        <v>33</v>
-      </c>
-      <c r="T5" t="n">
-        <v>18</v>
-      </c>
-      <c r="U5" t="n">
-        <v>51</v>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="W5" t="n">
-        <v>21</v>
-      </c>
-      <c r="X5" t="n">
-        <v>33</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>54</v>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="AA5" t="n">
-        <v>39</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>27</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>66</v>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="AE5" t="n">
-        <v>25</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>41</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>66</v>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="AI5" t="n">
-        <v>37</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>29</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>66</v>
-      </c>
-      <c r="AL5" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1AM18CS028</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>20</v>
-      </c>
-      <c r="D6" t="n">
-        <v>21</v>
-      </c>
-      <c r="E6" t="n">
-        <v>41</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>21</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>21</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>22</v>
-      </c>
-      <c r="L6" t="n">
-        <v>8</v>
-      </c>
-      <c r="M6" t="n">
-        <v>30</v>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="O6" t="n">
-        <v>18</v>
-      </c>
-      <c r="P6" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>33</v>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="S6" t="n">
-        <v>19</v>
-      </c>
-      <c r="T6" t="n">
-        <v>9</v>
-      </c>
-      <c r="U6" t="n">
-        <v>28</v>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="W6" t="n">
-        <v>17</v>
-      </c>
-      <c r="X6" t="n">
-        <v>9</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>26</v>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="AA6" t="n">
-        <v>33</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>27</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>60</v>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="AE6" t="n">
-        <v>25</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>38</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>63</v>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="AI6" t="n">
-        <v>37</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>26</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>63</v>
-      </c>
-      <c r="AL6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>